<commit_message>
Added feature to take metabolite concentrations from data file
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_putida_v3.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/true_res_putida_v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2233,7 +2233,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2960,7 +2960,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3714,8 +3714,8 @@
   </sheetPr>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L40" activeCellId="0" sqref="L40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L40" activeCellId="1" sqref="A45:C52 L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5577,7 +5577,7 @@
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13504,7 +13504,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14415,7 +14415,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15178,7 +15178,7 @@
   <dimension ref="A2:A51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15455,7 +15455,7 @@
   <dimension ref="A2:A53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15742,7 +15742,7 @@
   <dimension ref="A2:A53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16029,7 +16029,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A45:C52 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16605,8 +16605,8 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="A45:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17098,92 +17098,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0</v>
+        <v>1E-012</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>